<commit_message>
UI Overhaul - Major rewrite of the user interface - started to replace some art and assets - updated the progress bar implementation - changed the stats implementation for players and monsters - started to move some save state into the new saving class
</commit_message>
<xml_diff>
--- a/data/content/Mercenaries.xlsx
+++ b/data/content/Mercenaries.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mercenaries" sheetId="2" r:id="rId1"/>
     <sheet name="Upgrades" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -34,12 +34,6 @@
     <t>icon</t>
   </si>
   <si>
-    <t>costPower</t>
-  </si>
-  <si>
-    <t>upgradeType</t>
-  </si>
-  <si>
     <t>trnFoot1</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Warlock</t>
   </si>
   <si>
-    <t>baseGps</t>
-  </si>
-  <si>
     <t>hp5Mult</t>
   </si>
   <si>
@@ -139,27 +130,15 @@
     <t>spdMult</t>
   </si>
   <si>
-    <t>evaMult</t>
-  </si>
-  <si>
     <t>critDmgMult</t>
   </si>
   <si>
-    <t>basePrice</t>
-  </si>
-  <si>
-    <t>baseAps</t>
-  </si>
-  <si>
     <t>requiredMerc</t>
   </si>
   <si>
     <t>requiredAmount</t>
   </si>
   <si>
-    <t>gpsMult</t>
-  </si>
-  <si>
     <t>footMan</t>
   </si>
   <si>
@@ -194,6 +173,18 @@
   </si>
   <si>
     <t>iconMercWarlock.png</t>
+  </si>
+  <si>
+    <t>evaRatingMult</t>
+  </si>
+  <si>
+    <t>gps</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>goldMult</t>
   </si>
 </sst>
 </file>
@@ -587,25 +578,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,172 +605,151 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1.05</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>1.05</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>360</v>
+      </c>
+      <c r="D4">
+        <v>4000</v>
+      </c>
+      <c r="G4">
+        <v>1.05</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <v>0.1</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>6800</v>
+      </c>
+      <c r="D5">
+        <v>80000</v>
+      </c>
+      <c r="H5">
         <v>1.05</v>
       </c>
-      <c r="L2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>0.1</v>
-      </c>
-      <c r="D3">
-        <v>0.94</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="G3">
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>128000</v>
+      </c>
+      <c r="D6">
+        <v>1600000</v>
+      </c>
+      <c r="I6">
         <v>1.05</v>
       </c>
-      <c r="L3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
-      </c>
-      <c r="D4">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E4">
-        <v>4000</v>
-      </c>
-      <c r="H4">
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>2400000</v>
+      </c>
+      <c r="D7">
+        <v>32000000</v>
+      </c>
+      <c r="J7">
         <v>1.05</v>
       </c>
-      <c r="L4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>83</v>
-      </c>
-      <c r="E5">
-        <v>80000</v>
-      </c>
-      <c r="I5">
-        <v>1.05</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="K7" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6">
-        <v>0.1</v>
-      </c>
-      <c r="D6">
-        <v>780</v>
-      </c>
-      <c r="E6">
-        <v>1600000</v>
-      </c>
-      <c r="J6">
-        <v>1.05</v>
-      </c>
-      <c r="L6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
-      </c>
-      <c r="D7">
-        <v>7339</v>
-      </c>
-      <c r="E7">
-        <v>32000000</v>
-      </c>
-      <c r="K7">
-        <v>1.05</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -791,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,10 +772,9 @@
     <col min="2" max="2" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
@@ -822,17 +792,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="E1" t="s">
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="J1"/>
       <c r="K1"/>
@@ -841,28 +808,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
         <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
       </c>
       <c r="J2"/>
       <c r="K2"/>
@@ -871,28 +835,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1">
         <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>20</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
@@ -901,28 +862,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1">
         <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -931,28 +889,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1">
         <v>49</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>50</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -961,158 +916,140 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>75</v>
+      </c>
+      <c r="G6" s="1">
         <v>74</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1">
         <v>99</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>150</v>
+      </c>
+      <c r="G8" s="1">
         <v>149</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>200</v>
+      </c>
+      <c r="G9" s="1">
         <v>199</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>250</v>
+      </c>
+      <c r="G10" s="1">
         <v>249</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>300</v>
+      </c>
+      <c r="G11" s="1">
         <v>299</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mercenary update part 3 - Mercenaries are functional enough for now, still not applying stats - Updated the currency display and gave it a separate dialog - Removed all legacy mercenary code - Fixed issues reported by closure - Renamed static to staticData since it conflicts with the reserved keyword static - adjusted style sheets and made use of the new include from crystal build - ensured panels and dialogs are only draggable on the header - added support for showing the currency influx and affordable / not affordable on currencyControl
</commit_message>
<xml_diff>
--- a/data/content/Mercenaries.xlsx
+++ b/data/content/Mercenaries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="Mercenaries" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -121,9 +121,6 @@
     <t>hp5Mult</t>
   </si>
   <si>
-    <t>hpMult</t>
-  </si>
-  <si>
     <t>dmgMult</t>
   </si>
   <si>
@@ -185,6 +182,18 @@
   </si>
   <si>
     <t>goldMult</t>
+  </si>
+  <si>
+    <t>xps</t>
+  </si>
+  <si>
+    <t>hp5</t>
+  </si>
+  <si>
+    <t>mp5</t>
+  </si>
+  <si>
+    <t>hpMaxMult</t>
   </si>
 </sst>
 </file>
@@ -578,26 +587,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,148 +618,157 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
         <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>1.05</v>
       </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>4000</v>
       </c>
       <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="I3">
         <v>1.05</v>
       </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
       <c r="C4">
-        <v>360</v>
+        <v>80000</v>
       </c>
       <c r="D4">
-        <v>4000</v>
-      </c>
-      <c r="G4">
+        <v>210</v>
+      </c>
+      <c r="J4">
         <v>1.05</v>
       </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
       <c r="C5">
-        <v>6800</v>
+        <v>1500000</v>
       </c>
       <c r="D5">
-        <v>80000</v>
-      </c>
-      <c r="H5">
+        <v>3500</v>
+      </c>
+      <c r="K5">
         <v>1.05</v>
       </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
       <c r="C6">
-        <v>128000</v>
+        <v>34000000</v>
       </c>
       <c r="D6">
-        <v>1600000</v>
-      </c>
-      <c r="I6">
+        <v>73000</v>
+      </c>
+      <c r="L6">
         <v>1.05</v>
       </c>
-      <c r="K6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7">
-        <v>2400000</v>
+        <v>670000000</v>
       </c>
       <c r="D7">
-        <v>32000000</v>
-      </c>
-      <c r="J7">
+        <v>1200000</v>
+      </c>
+      <c r="M7">
         <v>1.05</v>
       </c>
-      <c r="K7" t="s">
-        <v>50</v>
+      <c r="N7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -793,13 +812,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J1"/>
       <c r="K1"/>

</xml_diff>

<commit_message>
Bugfix and Release / Debug Config - Fixed mercenary icon root - Fixed exception in Save doGetSize when accessing localStorage for the first time - Made a separate Release config and updated the html to use the web versions of jquery for that - Updated version of CrystalBuild
</commit_message>
<xml_diff>
--- a/data/content/Mercenaries.xlsx
+++ b/data/content/Mercenaries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766"/>
+    <workbookView xWindow="12090" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="Mercenaries" sheetId="2" r:id="rId1"/>
@@ -154,24 +154,6 @@
     <t>warlock</t>
   </si>
   <si>
-    <t>iconMercFootMan.png</t>
-  </si>
-  <si>
-    <t>iconMercCleric.png</t>
-  </si>
-  <si>
-    <t>iconMercCommander.png</t>
-  </si>
-  <si>
-    <t>iconMercMage.png</t>
-  </si>
-  <si>
-    <t>iconMercAssassin.png</t>
-  </si>
-  <si>
-    <t>iconMercWarlock.png</t>
-  </si>
-  <si>
     <t>evaRatingMult</t>
   </si>
   <si>
@@ -194,6 +176,24 @@
   </si>
   <si>
     <t>hpMaxMult</t>
+  </si>
+  <si>
+    <t>mercFootMan.png</t>
+  </si>
+  <si>
+    <t>mercCleric.png</t>
+  </si>
+  <si>
+    <t>mercCommander.png</t>
+  </si>
+  <si>
+    <t>mercMage.png</t>
+  </si>
+  <si>
+    <t>mercAssassin.png</t>
+  </si>
+  <si>
+    <t>mercWarlock.png</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -615,19 +615,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>34</v>
@@ -636,13 +636,13 @@
         <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K1" t="s">
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M1" t="s">
         <v>35</v>
@@ -668,7 +668,7 @@
         <v>1.05</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>1.05</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>1.05</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>1.05</v>
       </c>
       <c r="N5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -748,7 +748,7 @@
         <v>1.05</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>1.05</v>
       </c>
       <c r="N7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +818,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J1"/>
       <c r="K1"/>

</xml_diff>